<commit_message>
change anode grid to big
</commit_message>
<xml_diff>
--- a/Geant_simulation/temp.xlsx
+++ b/Geant_simulation/temp.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>x pix</t>
   </si>
@@ -34,6 +34,24 @@
   </si>
   <si>
     <t>y res</t>
+  </si>
+  <si>
+    <t>N_emit</t>
+  </si>
+  <si>
+    <t>N_reg_tot</t>
+  </si>
+  <si>
+    <t>x_avr</t>
+  </si>
+  <si>
+    <t>y_avr</t>
+  </si>
+  <si>
+    <t>x_recon</t>
+  </si>
+  <si>
+    <t>y_recon</t>
   </si>
 </sst>
 </file>
@@ -82,6 +100,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -265,11 +286,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="93431296"/>
-        <c:axId val="93429760"/>
+        <c:axId val="371937752"/>
+        <c:axId val="371938144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93431296"/>
+        <c:axId val="371937752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -279,12 +300,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93429760"/>
+        <c:crossAx val="371938144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93429760"/>
+        <c:axId val="371938144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -295,14 +316,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93431296"/>
+        <c:crossAx val="371937752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -489,11 +509,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109704704"/>
-        <c:axId val="109703168"/>
+        <c:axId val="371938928"/>
+        <c:axId val="371939320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109704704"/>
+        <c:axId val="371938928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -503,12 +523,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109703168"/>
+        <c:crossAx val="371939320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109703168"/>
+        <c:axId val="371939320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -519,14 +539,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109704704"/>
+        <c:crossAx val="371938928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -651,11 +670,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115878528"/>
-        <c:axId val="115876992"/>
+        <c:axId val="371940104"/>
+        <c:axId val="373524408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115878528"/>
+        <c:axId val="371940104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -665,12 +684,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115876992"/>
+        <c:crossAx val="373524408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115876992"/>
+        <c:axId val="373524408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -681,14 +700,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115878528"/>
+        <c:crossAx val="371940104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -813,11 +831,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="95402624"/>
-        <c:axId val="95400704"/>
+        <c:axId val="373526760"/>
+        <c:axId val="373527152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95402624"/>
+        <c:axId val="373526760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -827,12 +845,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95400704"/>
+        <c:crossAx val="373527152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95400704"/>
+        <c:axId val="373527152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,14 +861,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95402624"/>
+        <c:crossAx val="373526760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1033,7 +1050,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1068,7 +1085,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2502,7 +2519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView topLeftCell="R1" workbookViewId="0">
       <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
@@ -3019,12 +3036,1766 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>-50</v>
+      </c>
+      <c r="C1">
+        <v>-50</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-40</v>
+      </c>
+      <c r="C2">
+        <v>-50</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>1600</v>
+      </c>
+      <c r="I2">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <v>0.45</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>-28.8276</v>
+      </c>
+      <c r="M2">
+        <v>-5.2413800000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>-30</v>
+      </c>
+      <c r="C3">
+        <v>-50</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>20.7273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-20</v>
+      </c>
+      <c r="C4">
+        <v>-50</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>-3.3043499999999999</v>
+      </c>
+      <c r="M4">
+        <v>6.6086999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-10</v>
+      </c>
+      <c r="C5">
+        <v>-50</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>10.1333</v>
+      </c>
+      <c r="M5">
+        <v>-5.0666700000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>-50</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>-50</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>-50</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>-50</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>-50</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11">
+        <v>-50</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>-50</v>
+      </c>
+      <c r="C12">
+        <v>-40</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>-40</v>
+      </c>
+      <c r="C13">
+        <v>-40</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>-30</v>
+      </c>
+      <c r="C14">
+        <v>-40</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>-20</v>
+      </c>
+      <c r="C15">
+        <v>-40</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>-10</v>
+      </c>
+      <c r="C16">
+        <v>-40</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>-40</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>-40</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>-40</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <v>-40</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>40</v>
+      </c>
+      <c r="C21">
+        <v>-40</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>50</v>
+      </c>
+      <c r="C22">
+        <v>-40</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>-50</v>
+      </c>
+      <c r="C23">
+        <v>-30</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>-40</v>
+      </c>
+      <c r="C24">
+        <v>-30</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>-30</v>
+      </c>
+      <c r="C25">
+        <v>-30</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>-20</v>
+      </c>
+      <c r="C26">
+        <v>-30</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>-10</v>
+      </c>
+      <c r="C27">
+        <v>-30</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>-30</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>-30</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>-30</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>-30</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>40</v>
+      </c>
+      <c r="C32">
+        <v>-30</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>50</v>
+      </c>
+      <c r="C33">
+        <v>-30</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>-50</v>
+      </c>
+      <c r="C34">
+        <v>-20</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>-40</v>
+      </c>
+      <c r="C35">
+        <v>-20</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>-30</v>
+      </c>
+      <c r="C36">
+        <v>-20</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>-20</v>
+      </c>
+      <c r="C37">
+        <v>-20</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>-10</v>
+      </c>
+      <c r="C38">
+        <v>-20</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>-20</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>-20</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>20</v>
+      </c>
+      <c r="C41">
+        <v>-20</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>30</v>
+      </c>
+      <c r="C42">
+        <v>-20</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>40</v>
+      </c>
+      <c r="C43">
+        <v>-20</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>50</v>
+      </c>
+      <c r="C44">
+        <v>-20</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>-50</v>
+      </c>
+      <c r="C45">
+        <v>-10</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>-40</v>
+      </c>
+      <c r="C46">
+        <v>-10</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>-30</v>
+      </c>
+      <c r="C47">
+        <v>-10</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>-20</v>
+      </c>
+      <c r="C48">
+        <v>-10</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>-10</v>
+      </c>
+      <c r="C49">
+        <v>-10</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>-10</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>-10</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>20</v>
+      </c>
+      <c r="C52">
+        <v>-10</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>30</v>
+      </c>
+      <c r="C53">
+        <v>-10</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>40</v>
+      </c>
+      <c r="C54">
+        <v>-10</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>50</v>
+      </c>
+      <c r="C55">
+        <v>-10</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>-50</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>-40</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>-30</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>-20</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>-10</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>10</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>20</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>30</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>40</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>50</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>-50</v>
+      </c>
+      <c r="C67">
+        <v>10</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>-40</v>
+      </c>
+      <c r="C68">
+        <v>10</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>-30</v>
+      </c>
+      <c r="C69">
+        <v>10</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>-20</v>
+      </c>
+      <c r="C70">
+        <v>10</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>-10</v>
+      </c>
+      <c r="C71">
+        <v>10</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>10</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>10</v>
+      </c>
+      <c r="C73">
+        <v>10</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>20</v>
+      </c>
+      <c r="C74">
+        <v>10</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>30</v>
+      </c>
+      <c r="C75">
+        <v>10</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>40</v>
+      </c>
+      <c r="C76">
+        <v>10</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>50</v>
+      </c>
+      <c r="C77">
+        <v>10</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>-50</v>
+      </c>
+      <c r="C78">
+        <v>20</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>-40</v>
+      </c>
+      <c r="C79">
+        <v>20</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>-30</v>
+      </c>
+      <c r="C80">
+        <v>20</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>-20</v>
+      </c>
+      <c r="C81">
+        <v>20</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>-10</v>
+      </c>
+      <c r="C82">
+        <v>20</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>20</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>20</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>20</v>
+      </c>
+      <c r="C85">
+        <v>20</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>30</v>
+      </c>
+      <c r="C86">
+        <v>20</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>40</v>
+      </c>
+      <c r="C87">
+        <v>20</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>50</v>
+      </c>
+      <c r="C88">
+        <v>20</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>-50</v>
+      </c>
+      <c r="C89">
+        <v>30</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>-40</v>
+      </c>
+      <c r="C90">
+        <v>30</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>-30</v>
+      </c>
+      <c r="C91">
+        <v>30</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>-20</v>
+      </c>
+      <c r="C92">
+        <v>30</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>-10</v>
+      </c>
+      <c r="C93">
+        <v>30</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>30</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>10</v>
+      </c>
+      <c r="C95">
+        <v>30</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>20</v>
+      </c>
+      <c r="C96">
+        <v>30</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>30</v>
+      </c>
+      <c r="C97">
+        <v>30</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>40</v>
+      </c>
+      <c r="C98">
+        <v>30</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>50</v>
+      </c>
+      <c r="C99">
+        <v>30</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>-50</v>
+      </c>
+      <c r="C100">
+        <v>40</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>-40</v>
+      </c>
+      <c r="C101">
+        <v>40</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>-30</v>
+      </c>
+      <c r="C102">
+        <v>40</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>-20</v>
+      </c>
+      <c r="C103">
+        <v>40</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>-10</v>
+      </c>
+      <c r="C104">
+        <v>40</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+      <c r="C105">
+        <v>40</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>10</v>
+      </c>
+      <c r="C106">
+        <v>40</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107">
+        <v>20</v>
+      </c>
+      <c r="C107">
+        <v>40</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <v>30</v>
+      </c>
+      <c r="C108">
+        <v>40</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>40</v>
+      </c>
+      <c r="C109">
+        <v>40</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <v>50</v>
+      </c>
+      <c r="C110">
+        <v>40</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <v>-50</v>
+      </c>
+      <c r="C111">
+        <v>50</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <v>-40</v>
+      </c>
+      <c r="C112">
+        <v>50</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>-30</v>
+      </c>
+      <c r="C113">
+        <v>50</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <v>-20</v>
+      </c>
+      <c r="C114">
+        <v>50</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <v>-10</v>
+      </c>
+      <c r="C115">
+        <v>50</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>50</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>10</v>
+      </c>
+      <c r="C117">
+        <v>50</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>20</v>
+      </c>
+      <c r="C118">
+        <v>50</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <v>30</v>
+      </c>
+      <c r="C119">
+        <v>50</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <v>40</v>
+      </c>
+      <c r="C120">
+        <v>50</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>50</v>
+      </c>
+      <c r="C121">
+        <v>50</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>